<commit_message>
automation cho chức năng update
</commit_message>
<xml_diff>
--- a/src/Data/Login.xlsx
+++ b/src/Data/Login.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Java\src\JaVaTestAppium\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963CD78-7415-4A11-BE5B-0813E48B5803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B878A0D7-EA32-4513-B93C-D4359A09D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4236" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{F893E997-8251-44C5-9FC1-92383C03822B}"/>
+    <workbookView xWindow="4236" yWindow="2244" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{F893E997-8251-44C5-9FC1-92383C03822B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>nhuyyy@gmail.com</t>
   </si>
@@ -42,6 +43,15 @@
   </si>
   <si>
     <t>invalid</t>
+  </si>
+  <si>
+    <t>xem phim</t>
+  </si>
+  <si>
+    <t>xem</t>
+  </si>
+  <si>
+    <t>hai</t>
   </si>
 </sst>
 </file>
@@ -411,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C39D2F2-F80F-494B-8407-2C45F22731E6}">
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -471,4 +481,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35212CDE-5192-44B9-A16C-5A9E21EA79EB}">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="30.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="30.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>